<commit_message>
update grafico salud censal
</commit_message>
<xml_diff>
--- a/data/datos_tp.xlsx
+++ b/data/datos_tp.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\GitHub\indicadores-socioeconomicos\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://indecok-my.sharepoint.com/personal/agomezvargas_indec_gob_ar/Documents/Documentos/GitHub/indicadores-socioeconomicos/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26DABBFD-47B4-43E9-AE65-22DEBD3B4492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{26DABBFD-47B4-43E9-AE65-22DEBD3B4492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F95AC814-DBC3-4B61-9CD6-C1E1DA12F850}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1260" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{AF598439-62DC-4F7D-BE55-398D701C39E6}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="5" xr2:uid="{AF598439-62DC-4F7D-BE55-398D701C39E6}"/>
   </bookViews>
   <sheets>
     <sheet name="piramide" sheetId="9" r:id="rId1"/>
@@ -7314,7 +7314,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7530753F-476B-4D0D-BBB8-9652C24C5C79}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
@@ -8927,8 +8927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B6FAF5-E35B-4BBC-9459-CD58CEE31A92}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -9014,8 +9014,8 @@
         <v>37</v>
       </c>
       <c r="D6">
-        <f>93.31+6.5</f>
-        <v>99.81</v>
+        <f>92.31+1.19</f>
+        <v>93.5</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -9029,8 +9029,7 @@
         <v>37</v>
       </c>
       <c r="D7">
-        <f>100-D6</f>
-        <v>0.18999999999999773</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -9044,8 +9043,8 @@
         <v>36</v>
       </c>
       <c r="D8">
-        <f>92.28+6.76</f>
-        <v>99.04</v>
+        <f>92.28+0.96</f>
+        <v>93.24</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -9059,7 +9058,7 @@
         <v>36</v>
       </c>
       <c r="D9">
-        <v>0.96</v>
+        <v>6.76</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -9073,8 +9072,8 @@
         <v>37</v>
       </c>
       <c r="D10">
-        <f>92.05+6.05</f>
-        <v>98.1</v>
+        <f>92.06+1.89</f>
+        <v>93.95</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -9088,8 +9087,7 @@
         <v>37</v>
       </c>
       <c r="D11">
-        <f>100-D10</f>
-        <v>1.9000000000000057</v>
+        <v>6.05</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -9103,8 +9101,8 @@
         <v>36</v>
       </c>
       <c r="D12">
-        <f>92.29+6.1</f>
-        <v>98.39</v>
+        <f>92.29+1.61</f>
+        <v>93.9</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -9118,8 +9116,7 @@
         <v>36</v>
       </c>
       <c r="D13">
-        <f>100-D12</f>
-        <v>1.6099999999999994</v>
+        <v>6.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>